<commit_message>
Revision del cronograma de proyecto
</commit_message>
<xml_diff>
--- a/Desarrollo/SGVR/Gestión/SGVR_CP.xlsx
+++ b/Desarrollo/SGVR/Gestión/SGVR_CP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\G3-ACMSW\Desarrollo\SGVR\Gestión\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Terry\Documents\Maestria\G3-ACMSW\Desarrollo\SGVR\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6D524C-08C7-43CE-A0D9-4F24CE308F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B1832D-9B7C-48FD-8BBB-53C9425D8CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AA4BB2B9-CC80-4F61-B7B0-4C6847ED477F}"/>
+    <workbookView xWindow="15075" yWindow="3000" windowWidth="21555" windowHeight="14865" xr2:uid="{AA4BB2B9-CC80-4F61-B7B0-4C6847ED477F}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
@@ -922,7 +922,7 @@
   <dimension ref="B5:H42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1014,7 +1014,7 @@
         <v>44457</v>
       </c>
       <c r="H12" s="9">
-        <v>0.66</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
[UPD] - Se actualizó el porcentaje de avance del cronograma del proyecto
</commit_message>
<xml_diff>
--- a/Desarrollo/SGVR/Gestión/SGVR_CP.xlsx
+++ b/Desarrollo/SGVR/Gestión/SGVR_CP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Terry\Documents\Maestria\G3-ACMSW\Desarrollo\SGVR\Gestión\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maestria\Ciclo 04\Administración de la Configuración y Mantenimiento de SW\Trabajo final\G3-ACMSW\Desarrollo\SGVR\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B1832D-9B7C-48FD-8BBB-53C9425D8CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614B8940-7151-4BDE-A2B7-14A0CD8A822C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15075" yWindow="3000" windowWidth="21555" windowHeight="14865" xr2:uid="{AA4BB2B9-CC80-4F61-B7B0-4C6847ED477F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AA4BB2B9-CC80-4F61-B7B0-4C6847ED477F}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
@@ -577,7 +577,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>1683</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>129989</xdr:rowOff>
+      <xdr:rowOff>133799</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -921,23 +921,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EC8E214-110B-4268-B8E8-EAB6D71E9750}">
   <dimension ref="B5:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" style="1" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="52.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" style="5" customWidth="1"/>
-    <col min="6" max="7" width="11.42578125" style="4"/>
-    <col min="8" max="8" width="14.42578125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="42.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="52.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="34.5546875" style="5" customWidth="1"/>
+    <col min="6" max="7" width="11.44140625" style="4"/>
+    <col min="8" max="8" width="14.44140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -945,7 +945,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
@@ -953,12 +953,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C7" s="12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C8" s="13" t="s">
         <v>47</v>
       </c>
@@ -966,12 +966,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H9" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>4</v>
       </c>
@@ -994,7 +994,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>76</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>11</v>
       </c>
@@ -1037,10 +1037,10 @@
         <v>44460</v>
       </c>
       <c r="H13" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>81</v>
       </c>
@@ -1060,10 +1060,10 @@
         <v>44460</v>
       </c>
       <c r="H14" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>12</v>
       </c>
@@ -1083,10 +1083,10 @@
         <v>44460</v>
       </c>
       <c r="H15" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>54</v>
       </c>
@@ -1097,7 +1097,7 @@
       <c r="G16" s="19"/>
       <c r="H16" s="20"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>13</v>
       </c>
@@ -1117,10 +1117,10 @@
         <v>44463</v>
       </c>
       <c r="H17" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>14</v>
       </c>
@@ -1140,10 +1140,10 @@
         <v>44463</v>
       </c>
       <c r="H18" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>15</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="15" t="s">
         <v>79</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="18" t="s">
         <v>16</v>
       </c>
@@ -1200,7 +1200,7 @@
       <c r="G21" s="19"/>
       <c r="H21" s="20"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
         <v>37</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
         <v>38</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
         <v>39</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>20</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="15" t="s">
         <v>79</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="18" t="s">
         <v>21</v>
       </c>
@@ -1326,7 +1326,7 @@
       <c r="G27" s="19"/>
       <c r="H27" s="20"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
         <v>22</v>
       </c>
@@ -1349,7 +1349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
         <v>23</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
         <v>24</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="7" t="s">
         <v>25</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="15" t="s">
         <v>79</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
         <v>26</v>
       </c>
@@ -1452,7 +1452,7 @@
       <c r="G33" s="19"/>
       <c r="H33" s="20"/>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="7" t="s">
         <v>50</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="7" t="s">
         <v>27</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="7" t="s">
         <v>28</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="7" t="s">
         <v>29</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="15" t="s">
         <v>79</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="18" t="s">
         <v>30</v>
       </c>
@@ -1578,7 +1578,7 @@
       <c r="G39" s="19"/>
       <c r="H39" s="20"/>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="7" t="s">
         <v>31</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="7" t="s">
         <v>32</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="15" t="s">
         <v>79</v>
       </c>
@@ -1669,16 +1669,16 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>91</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="7">
         <v>1</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="7">
         <v>2</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="7">
         <v>3</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="7">
         <v>4</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="7">
         <v>5</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
         <v>6</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
         <v>7</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="7">
         <v>8</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
         <v>9</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
         <v>10</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="7">
         <v>11</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="7">
         <v>12</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="7">
         <v>13</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="7">
         <v>14</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="7">
         <v>15</v>
       </c>
@@ -1950,7 +1950,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="7">
         <v>16</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="7">
         <v>17</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="7">
         <v>18</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="7">
         <v>19</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="7">
         <v>20</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="7">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
[FIX] - Actualización del avance del cronograma de proyecto para la finalización del sprint 1
</commit_message>
<xml_diff>
--- a/Desarrollo/SGVR/Gestión/SGVR_CP.xlsx
+++ b/Desarrollo/SGVR/Gestión/SGVR_CP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maestria\Ciclo 04\Administración de la Configuración y Mantenimiento de SW\Trabajo final\G3-ACMSW\Desarrollo\SGVR\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614B8940-7151-4BDE-A2B7-14A0CD8A822C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8E2878-AFEB-4184-8570-48B17C378CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AA4BB2B9-CC80-4F61-B7B0-4C6847ED477F}"/>
+    <workbookView xWindow="-216" yWindow="0" windowWidth="23256" windowHeight="12480" xr2:uid="{AA4BB2B9-CC80-4F61-B7B0-4C6847ED477F}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
@@ -922,7 +922,7 @@
   <dimension ref="B5:H42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="B21" sqref="B21:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1117,7 +1117,7 @@
         <v>44463</v>
       </c>
       <c r="H17" s="9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -1140,7 +1140,7 @@
         <v>44463</v>
       </c>
       <c r="H18" s="9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -1163,7 +1163,7 @@
         <v>44465</v>
       </c>
       <c r="H19" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -1186,7 +1186,7 @@
         <v>44465</v>
       </c>
       <c r="H20" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[FIX] - Se agregó el documento de requerimientos no funcionales, se dejó en un 50% el documento de Actas de pruebas de calidad y se actualizó el cronograma de proyecto
</commit_message>
<xml_diff>
--- a/Desarrollo/SGVR/Gestión/SGVR_CP.xlsx
+++ b/Desarrollo/SGVR/Gestión/SGVR_CP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maestria\Ciclo 04\Administración de la Configuración y Mantenimiento de SW\Trabajo final\G3-ACMSW\Desarrollo\SGVR\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8E2878-AFEB-4184-8570-48B17C378CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC24265-20FE-4227-AC4D-9406671BB209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-216" yWindow="0" windowWidth="23256" windowHeight="12480" xr2:uid="{AA4BB2B9-CC80-4F61-B7B0-4C6847ED477F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AA4BB2B9-CC80-4F61-B7B0-4C6847ED477F}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
@@ -921,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EC8E214-110B-4268-B8E8-EAB6D71E9750}">
   <dimension ref="B5:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:H21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1266,7 +1266,7 @@
         <v>44468</v>
       </c>
       <c r="H24" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -1289,7 +1289,7 @@
         <v>44469</v>
       </c>
       <c r="H25" s="9">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[FIX] - Actualización en los documentos de cronograma de proyecto y plan de gestión de la configuración
</commit_message>
<xml_diff>
--- a/Desarrollo/SGVR/Gestión/SGVR_CP.xlsx
+++ b/Desarrollo/SGVR/Gestión/SGVR_CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maestria\Ciclo 04\Administración de la Configuración y Mantenimiento de SW\Trabajo final\G3-ACMSW\Desarrollo\SGVR\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC24265-20FE-4227-AC4D-9406671BB209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A3D74C-B0B9-4B24-A1F3-7906487776C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AA4BB2B9-CC80-4F61-B7B0-4C6847ED477F}"/>
   </bookViews>
@@ -922,7 +922,7 @@
   <dimension ref="B5:H42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="B27" sqref="B27:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1220,7 +1220,7 @@
         <v>44468</v>
       </c>
       <c r="H22" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -1243,7 +1243,7 @@
         <v>44468</v>
       </c>
       <c r="H23" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -1289,7 +1289,7 @@
         <v>44469</v>
       </c>
       <c r="H25" s="9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -1312,7 +1312,7 @@
         <v>44469</v>
       </c>
       <c r="H26" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[UPD] - Actualizando cronograma de proyecto
</commit_message>
<xml_diff>
--- a/Desarrollo/SGVR/Gestión/SGVR_CP.xlsx
+++ b/Desarrollo/SGVR/Gestión/SGVR_CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maestria\Ciclo 04\Administración de la Configuración y Mantenimiento de SW\Trabajo final\G3-ACMSW\Desarrollo\SGVR\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A3D74C-B0B9-4B24-A1F3-7906487776C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6F507D-C4C0-4D24-85A1-F515EEC7E904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AA4BB2B9-CC80-4F61-B7B0-4C6847ED477F}"/>
   </bookViews>
@@ -20,6 +20,13 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -921,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EC8E214-110B-4268-B8E8-EAB6D71E9750}">
   <dimension ref="B5:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:H27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1346,7 +1353,7 @@
         <v>44472</v>
       </c>
       <c r="H28" s="9">
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -1369,7 +1376,7 @@
         <v>44475</v>
       </c>
       <c r="H29" s="9">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[UPD] - Actualización de cronograma de proyectos
</commit_message>
<xml_diff>
--- a/Desarrollo/SGVR/Gestión/SGVR_CP.xlsx
+++ b/Desarrollo/SGVR/Gestión/SGVR_CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maestria\Ciclo 04\Administración de la Configuración y Mantenimiento de SW\Trabajo final\G3-ACMSW\Desarrollo\SGVR\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6F507D-C4C0-4D24-85A1-F515EEC7E904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43335AFB-9CF8-4843-A485-CC9B90F46A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AA4BB2B9-CC80-4F61-B7B0-4C6847ED477F}"/>
   </bookViews>
@@ -929,7 +929,7 @@
   <dimension ref="B5:H42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1399,7 +1399,7 @@
         <v>44479</v>
       </c>
       <c r="H30" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[UPD] - Actualización de cronograma de proyecto
</commit_message>
<xml_diff>
--- a/Desarrollo/SGVR/Gestión/SGVR_CP.xlsx
+++ b/Desarrollo/SGVR/Gestión/SGVR_CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maestria\Ciclo 04\Administración de la Configuración y Mantenimiento de SW\Trabajo final\G3-ACMSW\Desarrollo\SGVR\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43335AFB-9CF8-4843-A485-CC9B90F46A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330D3FC8-639C-4945-986D-4E2A1ED342B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AA4BB2B9-CC80-4F61-B7B0-4C6847ED477F}"/>
   </bookViews>
@@ -929,7 +929,7 @@
   <dimension ref="B5:H42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="B33" sqref="B33:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1353,7 +1353,7 @@
         <v>44472</v>
       </c>
       <c r="H28" s="9">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -1376,7 +1376,7 @@
         <v>44475</v>
       </c>
       <c r="H29" s="9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -1422,7 +1422,7 @@
         <v>44485</v>
       </c>
       <c r="H31" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
@@ -1445,7 +1445,7 @@
         <v>44485</v>
       </c>
       <c r="H32" s="9">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
@@ -1673,7 +1673,7 @@
   <dimension ref="B2:F23"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[UPD] - Actualizando item "Cronograma de Proyecto"
</commit_message>
<xml_diff>
--- a/Desarrollo/SGVR/Gestión/SGVR_CP.xlsx
+++ b/Desarrollo/SGVR/Gestión/SGVR_CP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maestria\Ciclo 04\Administración de la Configuración y Mantenimiento de SW\Trabajo final\G3-ACMSW\Desarrollo\SGVR\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{330D3FC8-639C-4945-986D-4E2A1ED342B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD99D671-DBEF-419E-AAFD-CB5E6235E1D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AA4BB2B9-CC80-4F61-B7B0-4C6847ED477F}"/>
   </bookViews>
@@ -928,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EC8E214-110B-4268-B8E8-EAB6D71E9750}">
   <dimension ref="B5:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:H33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39:H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1445,7 +1445,7 @@
         <v>44485</v>
       </c>
       <c r="H32" s="9">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
@@ -1479,7 +1479,7 @@
         <v>44496</v>
       </c>
       <c r="H34" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
@@ -1502,7 +1502,7 @@
         <v>44499</v>
       </c>
       <c r="H35" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
@@ -1525,7 +1525,7 @@
         <v>44506</v>
       </c>
       <c r="H36" s="9">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[UPD] - Se actualizó item de cronograma de proyecto
</commit_message>
<xml_diff>
--- a/Desarrollo/SGVR/Gestión/SGVR_CP.xlsx
+++ b/Desarrollo/SGVR/Gestión/SGVR_CP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maestria\Ciclo 04\Administración de la Configuración y Mantenimiento de SW\Trabajo final\G3-ACMSW\Desarrollo\SGVR\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD99D671-DBEF-419E-AAFD-CB5E6235E1D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BE5D4D-E0A0-4090-9F1F-FC86236785FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AA4BB2B9-CC80-4F61-B7B0-4C6847ED477F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{AA4BB2B9-CC80-4F61-B7B0-4C6847ED477F}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
@@ -928,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EC8E214-110B-4268-B8E8-EAB6D71E9750}">
   <dimension ref="B5:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39:H39"/>
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1525,7 +1525,7 @@
         <v>44506</v>
       </c>
       <c r="H36" s="9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
@@ -1548,7 +1548,7 @@
         <v>44512</v>
       </c>
       <c r="H37" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
@@ -1672,8 +1672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CFFB9D0-D817-4566-A111-088BEC4AD802}">
   <dimension ref="B2:F23"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
[UPD] - Actualizando item de cronograma del proyecto
</commit_message>
<xml_diff>
--- a/Desarrollo/SGVR/Gestión/SGVR_CP.xlsx
+++ b/Desarrollo/SGVR/Gestión/SGVR_CP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Terry\Documents\Maestria\G3-ACMSW\Desarrollo\SGVR\Gestión\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maestria\Ciclo 04\Administración de la Configuración y Mantenimiento de SW\Trabajo final\G3-ACMSW\Desarrollo\SGVR\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DD01E8-E069-4C56-A413-89FA3C6E7D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE3F5C4-642E-4327-A0E4-D0D2816F3DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8625" yWindow="6735" windowWidth="21270" windowHeight="9375" xr2:uid="{AA4BB2B9-CC80-4F61-B7B0-4C6847ED477F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AA4BB2B9-CC80-4F61-B7B0-4C6847ED477F}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="100">
   <si>
     <t>Escuela de Posgrado</t>
   </si>
@@ -333,9 +333,6 @@
   </si>
   <si>
     <t>XLSX</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -929,25 +926,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EC8E214-110B-4268-B8E8-EAB6D71E9750}">
-  <dimension ref="B5:H44"/>
+  <dimension ref="B5:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" style="1" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="52.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" style="5" customWidth="1"/>
-    <col min="6" max="7" width="11.42578125" style="4"/>
-    <col min="8" max="8" width="14.42578125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="42.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="52.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="34.5546875" style="5" customWidth="1"/>
+    <col min="6" max="7" width="11.44140625" style="4"/>
+    <col min="8" max="8" width="14.44140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:8" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -955,7 +952,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
@@ -963,12 +960,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C7" s="12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C8" s="13" t="s">
         <v>47</v>
       </c>
@@ -976,12 +973,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H9" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>4</v>
       </c>
@@ -1004,7 +1001,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="7" t="s">
         <v>76</v>
       </c>
@@ -1027,7 +1024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>11</v>
       </c>
@@ -1050,7 +1047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>81</v>
       </c>
@@ -1073,7 +1070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
         <v>12</v>
       </c>
@@ -1096,7 +1093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>54</v>
       </c>
@@ -1107,7 +1104,7 @@
       <c r="G16" s="19"/>
       <c r="H16" s="20"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="7" t="s">
         <v>13</v>
       </c>
@@ -1130,7 +1127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>14</v>
       </c>
@@ -1153,7 +1150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>15</v>
       </c>
@@ -1176,7 +1173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="15" t="s">
         <v>79</v>
       </c>
@@ -1199,7 +1196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="18" t="s">
         <v>16</v>
       </c>
@@ -1210,7 +1207,7 @@
       <c r="G21" s="19"/>
       <c r="H21" s="20"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
         <v>37</v>
       </c>
@@ -1233,7 +1230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="7" t="s">
         <v>38</v>
       </c>
@@ -1256,7 +1253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="7" t="s">
         <v>39</v>
       </c>
@@ -1279,7 +1276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>20</v>
       </c>
@@ -1302,7 +1299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="15" t="s">
         <v>79</v>
       </c>
@@ -1325,7 +1322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="18" t="s">
         <v>21</v>
       </c>
@@ -1336,7 +1333,7 @@
       <c r="G27" s="19"/>
       <c r="H27" s="20"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="7" t="s">
         <v>22</v>
       </c>
@@ -1359,7 +1356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
         <v>23</v>
       </c>
@@ -1382,7 +1379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
         <v>24</v>
       </c>
@@ -1405,7 +1402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="7" t="s">
         <v>25</v>
       </c>
@@ -1428,7 +1425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="15" t="s">
         <v>79</v>
       </c>
@@ -1451,7 +1448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="18" t="s">
         <v>26</v>
       </c>
@@ -1462,7 +1459,7 @@
       <c r="G33" s="19"/>
       <c r="H33" s="20"/>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="7" t="s">
         <v>50</v>
       </c>
@@ -1485,7 +1482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="7" t="s">
         <v>27</v>
       </c>
@@ -1508,7 +1505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="7" t="s">
         <v>28</v>
       </c>
@@ -1531,7 +1528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="7" t="s">
         <v>29</v>
       </c>
@@ -1554,7 +1551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="15" t="s">
         <v>79</v>
       </c>
@@ -1577,7 +1574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="18" t="s">
         <v>30</v>
       </c>
@@ -1588,7 +1585,7 @@
       <c r="G39" s="19"/>
       <c r="H39" s="20"/>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="7" t="s">
         <v>31</v>
       </c>
@@ -1611,7 +1608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="7" t="s">
         <v>32</v>
       </c>
@@ -1631,10 +1628,10 @@
         <v>44519</v>
       </c>
       <c r="H41" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="15" t="s">
         <v>79</v>
       </c>
@@ -1655,14 +1652,6 @@
       </c>
       <c r="H42" s="9">
         <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B44" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1687,16 +1676,16 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>91</v>
       </c>
@@ -1713,7 +1702,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="7">
         <v>1</v>
       </c>
@@ -1730,7 +1719,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="7">
         <v>2</v>
       </c>
@@ -1747,7 +1736,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="7">
         <v>3</v>
       </c>
@@ -1764,7 +1753,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="7">
         <v>4</v>
       </c>
@@ -1781,7 +1770,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="7">
         <v>5</v>
       </c>
@@ -1798,7 +1787,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
         <v>6</v>
       </c>
@@ -1815,7 +1804,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
         <v>7</v>
       </c>
@@ -1832,7 +1821,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="7">
         <v>8</v>
       </c>
@@ -1849,7 +1838,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
         <v>9</v>
       </c>
@@ -1866,7 +1855,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
         <v>10</v>
       </c>
@@ -1883,7 +1872,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="7">
         <v>11</v>
       </c>
@@ -1900,7 +1889,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="7">
         <v>12</v>
       </c>
@@ -1917,7 +1906,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="7">
         <v>13</v>
       </c>
@@ -1934,7 +1923,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="7">
         <v>14</v>
       </c>
@@ -1951,7 +1940,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="7">
         <v>15</v>
       </c>
@@ -1968,7 +1957,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="7">
         <v>16</v>
       </c>
@@ -1985,7 +1974,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="7">
         <v>17</v>
       </c>
@@ -2002,7 +1991,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="7">
         <v>18</v>
       </c>
@@ -2019,7 +2008,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="7">
         <v>19</v>
       </c>
@@ -2036,7 +2025,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="7">
         <v>20</v>
       </c>
@@ -2053,7 +2042,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="7">
         <v>21</v>
       </c>

</xml_diff>